<commit_message>
Rebuilt the USGS service
</commit_message>
<xml_diff>
--- a/planning/TASKS_InstrumentToolkit.xlsx
+++ b/planning/TASKS_InstrumentToolkit.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Develop a general-purpose node for deriving an analyitical result from a voltage and calibration data.</t>
+  </si>
+  <si>
+    <t>Node to convert incoming DIY identifiers to a more descriptive value. (How can we get DIY metadata).</t>
+  </si>
+  <si>
+    <t>EnviroDIY publisher Source</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +608,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -615,7 +621,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="5">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
@@ -715,6 +721,17 @@
       <c r="D11" s="1"/>
       <c r="G11" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>